<commit_message>
change field in form hazop & report
</commit_message>
<xml_diff>
--- a/dotnet6-epha-api/wwwroot/AttachedFileTemp/HAZOP Report Template.xlsx
+++ b/dotnet6-epha-api/wwwroot/AttachedFileTemp/HAZOP Report Template.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dotnet6-epha-api\dotnet6-epha-api\wwwroot\AttachedFileTemp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18B89D0-4BA0-48CA-A9C9-AA0642019897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7336EB4-959D-42FA-8C02-13E92B008D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="597" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TrackTemplate" sheetId="32" r:id="rId1"/>
-    <sheet name="RecommTemplate" sheetId="37" r:id="rId2"/>
-    <sheet name="WorksheetTemplate" sheetId="36" r:id="rId3"/>
-    <sheet name="GuidewordsTemplate" sheetId="38" r:id="rId4"/>
-    <sheet name="SheetTemplate" sheetId="39" r:id="rId5"/>
+    <sheet name="HAZOP Cover Page" sheetId="41" r:id="rId1"/>
+    <sheet name="AttendeeSheetTemplate (2)" sheetId="43" r:id="rId2"/>
+    <sheet name="AttendeeSheetTemplate" sheetId="40" r:id="rId3"/>
+    <sheet name="TrackTemplate" sheetId="32" r:id="rId4"/>
+    <sheet name="RecommTemplate" sheetId="37" r:id="rId5"/>
+    <sheet name="WorksheetTemplate" sheetId="36" r:id="rId6"/>
+    <sheet name="GuidewordsTemplate" sheetId="38" r:id="rId7"/>
+    <sheet name="SheetTemplate" sheetId="39" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">GuidewordsTemplate!$A$1:$D$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">RecommTemplate!$A$1:$F$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TrackTemplate!$A$1:$F$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">WorksheetTemplate!$A$1:$O$14</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">GuidewordsTemplate!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">RecommTemplate!$1:$10</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">TrackTemplate!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">WorksheetTemplate!$1:$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">AttendeeSheetTemplate!$A$1:$O$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'AttendeeSheetTemplate (2)'!$A$1:$O$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">GuidewordsTemplate!$A$1:$D$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'HAZOP Cover Page'!$A$1:$L$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">RecommTemplate!$A$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">TrackTemplate!$A$1:$F$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">WorksheetTemplate!$A$1:$P$14</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">AttendeeSheetTemplate!$1:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'AttendeeSheetTemplate (2)'!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">GuidewordsTemplate!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'HAZOP Cover Page'!$1:$17</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">RecommTemplate!$1:$10</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">TrackTemplate!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">WorksheetTemplate!$1:$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>RECCOMENDATION STATUS TRACKING TABLE</t>
   </si>
@@ -230,12 +239,130 @@
   <si>
     <t>Area of Application</t>
   </si>
+  <si>
+    <t>HAZOP ATTENDEE SHEET &amp; HAZOP COVER PAGE</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Date of attendance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP PROJECT NO. : </t>
+  </si>
+  <si>
+    <t>CTCI PROJECT NO. :</t>
+  </si>
+  <si>
+    <t>HAZOP STUDY REPORT
+EPC MAIN WORK
+FOR 
+CFP CRUDE OIL TANK PROJECT</t>
+  </si>
+  <si>
+    <t>FOR FINAL</t>
+  </si>
+  <si>
+    <t>Thai Oil Public Company Limited</t>
+  </si>
+  <si>
+    <t>CERTIFIED</t>
+  </si>
+  <si>
+    <t>Issue For Final</t>
+  </si>
+  <si>
+    <t>PROJ.</t>
+  </si>
+  <si>
+    <t>Z0</t>
+  </si>
+  <si>
+    <t>Issue For Design</t>
+  </si>
+  <si>
+    <t>MGR.</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Issue For Review</t>
+  </si>
+  <si>
+    <t>Rev. 
+0</t>
+  </si>
+  <si>
+    <t>REV.</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>CHK.</t>
+  </si>
+  <si>
+    <t>APPR.</t>
+  </si>
+  <si>
+    <t>1 Mar 23</t>
+  </si>
+  <si>
+    <t>2 Mar 23</t>
+  </si>
+  <si>
+    <t>3 Mar 23</t>
+  </si>
+  <si>
+    <t>4 Mar 23</t>
+  </si>
+  <si>
+    <t>5 Mar 23</t>
+  </si>
+  <si>
+    <t>6 Mar 23</t>
+  </si>
+  <si>
+    <t>7 Mar 23</t>
+  </si>
+  <si>
+    <t>8 Mar 23</t>
+  </si>
+  <si>
+    <t>9 Mar 23</t>
+  </si>
+  <si>
+    <t>10 Mar 23</t>
+  </si>
+  <si>
+    <t>11 Mar 23</t>
+  </si>
+  <si>
+    <t>12 Mar 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">วัตถุประสงค์การศึกษาและขอบเขตงาน (Study Objective and Work Scope) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +428,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="42"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +461,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -508,11 +660,232 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -608,6 +981,178 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -681,6 +1226,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,6 +1344,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,13 +1389,92 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285424</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 14" descr="C:\Users\Sirachachp\AppData\Local\Microsoft\Windows\Temporary Internet Files\Content.Outlook\MM9BOPGC\Thaioil Corporate Logo (002).png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAEB836A-E5DC-44F3-8D19-E6CE1DB5A518}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6632986" y="9080799"/>
+          <a:ext cx="647598" cy="388172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>235325</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>71747</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>1026511</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>152877</xdr:rowOff>
@@ -1166,6 +1805,537 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C4F29D-EA86-4E57-A11D-FE94F4888AA3}">
+  <dimension ref="A1:L17"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" style="39" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="39" customWidth="1"/>
+    <col min="3" max="6" width="16.33203125" style="39" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="57" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" style="57" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="57" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="39" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="39" customWidth="1"/>
+    <col min="12" max="12" width="1.77734375" style="39" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="39" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="79"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="37"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="37"/>
+    </row>
+    <row r="3" spans="1:12" ht="179.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+    </row>
+    <row r="4" spans="1:12" ht="310.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" spans="1:12" ht="133.19999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+    </row>
+    <row r="6" spans="1:12" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="77"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" spans="1:12" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+    </row>
+    <row r="8" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="37"/>
+    </row>
+    <row r="9" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="37"/>
+    </row>
+    <row r="10" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="37"/>
+    </row>
+    <row r="11" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="37"/>
+    </row>
+    <row r="12" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="37"/>
+    </row>
+    <row r="13" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="49">
+        <v>0</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="37"/>
+    </row>
+    <row r="14" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="66"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="37"/>
+    </row>
+    <row r="15" spans="1:12" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="37"/>
+    </row>
+    <row r="16" spans="1:12" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="G8:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="G16:J16"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="71" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFD4A0-7FED-4EF0-9E39-989993D5603B}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" customWidth="1"/>
+    <col min="4" max="15" width="7.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="85"/>
+    </row>
+    <row r="2" spans="1:15" ht="246.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="155"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="157"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Angsana New,Bold"&amp;12QMTS-SFR-24, Rev. 00, 17/08/22&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1A60CB-7148-4EBE-88B8-4E11D6701992}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="Y26" sqref="Y26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" customWidth="1"/>
+    <col min="4" max="15" width="7.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="85"/>
+    </row>
+    <row r="2" spans="1:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
+      <c r="N2" s="89"/>
+      <c r="O2" s="90"/>
+    </row>
+    <row r="3" spans="1:15" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:O2"/>
+  </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="71" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Angsana New,Bold"&amp;12QMTS-SFR-24, Rev. 00, 17/08/22&amp;C&amp;"Angsana New,Bold"&amp;12Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1186,14 +2356,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="93"/>
     </row>
     <row r="2" spans="1:6" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1236,7 +2406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBADC2D-2F39-4DD0-9F8C-1B88F9D121D3}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -1253,167 +2423,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="93"/>
     </row>
     <row r="2" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="109"/>
     </row>
     <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="51"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="109"/>
     </row>
     <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="112"/>
     </row>
     <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="56"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="114"/>
       <c r="D5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="114"/>
     </row>
     <row r="6" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
     </row>
     <row r="7" spans="1:6" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="98"/>
     </row>
     <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="101"/>
     </row>
     <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="98"/>
     </row>
     <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
     </row>
     <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="98"/>
     </row>
     <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="97"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="98"/>
     </row>
     <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
     </row>
     <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="43"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
     </row>
     <row r="15" spans="1:6" ht="140.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
+      <c r="A15" s="102"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="103"/>
+      <c r="F15" s="104"/>
     </row>
     <row r="16" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="47" t="s">
+      <c r="C16" s="106"/>
+      <c r="D16" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="48"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1422,20 +2592,20 @@
       <c r="A17" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="95"/>
       <c r="F17" s="32"/>
     </row>
     <row r="18" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="95"/>
       <c r="F18" s="32"/>
     </row>
   </sheetData>
@@ -1472,12 +2642,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097ABC84-1B5E-489B-B95A-8609751415A0}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1491,12 +2661,13 @@
     <col min="10" max="10" width="32.109375" style="1" customWidth="1"/>
     <col min="11" max="13" width="4.5546875" style="27" customWidth="1"/>
     <col min="14" max="14" width="33" style="27" customWidth="1"/>
-    <col min="15" max="15" width="17.44140625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="15" width="6.5546875" style="27" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -1514,8 +2685,9 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1530,170 +2702,179 @@
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="92" t="s">
+      <c r="B3" s="151"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="153"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="76" t="s">
+      <c r="B4" s="135"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="135"/>
+      <c r="K4" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="77"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="90"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73" t="s">
+      <c r="L4" s="137"/>
+      <c r="M4" s="138"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="145"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="134"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="142"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="149"/>
+      <c r="O5" s="149"/>
+      <c r="P5" s="150"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="76" t="s">
+      <c r="B6" s="135"/>
+      <c r="C6" s="135"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="77"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="79"/>
-      <c r="L7" s="80"/>
-      <c r="M7" s="81"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="s">
+      <c r="L6" s="137"/>
+      <c r="M6" s="138"/>
+      <c r="N6" s="145"/>
+      <c r="O6" s="145"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="134"/>
+      <c r="B7" s="135"/>
+      <c r="C7" s="135"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="147"/>
+      <c r="O7" s="147"/>
+      <c r="P7" s="148"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="133" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="80"/>
-      <c r="M8" s="81"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="2"/>
-    </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="135"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="139"/>
+      <c r="L8" s="140"/>
+      <c r="M8" s="141"/>
+      <c r="N8" s="147"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="148"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="133"/>
+      <c r="B9" s="135"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="135"/>
+      <c r="E9" s="135"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="I9" s="135"/>
+      <c r="J9" s="135"/>
+      <c r="K9" s="142"/>
+      <c r="L9" s="143"/>
+      <c r="M9" s="144"/>
+      <c r="N9" s="149"/>
+      <c r="O9" s="149"/>
+      <c r="P9" s="150"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="62" t="s">
+      <c r="B10" s="119"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="122" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="63"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="2"/>
-    </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="123"/>
+      <c r="M10" s="124"/>
+      <c r="N10" s="125"/>
+      <c r="O10" s="125"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14"/>
@@ -1709,33 +2890,34 @@
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
+      <c r="P11" s="15"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="127" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="72"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="132"/>
       <c r="I12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="127" t="s">
         <v>23</v>
       </c>
       <c r="K12" s="18" t="s">
@@ -1743,18 +2925,21 @@
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
-      <c r="N12" s="68" t="s">
+      <c r="N12" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="115" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="117" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="127"/>
+      <c r="B13" s="127"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="127"/>
       <c r="E13" s="20" t="s">
         <v>28</v>
       </c>
@@ -1770,7 +2955,7 @@
       <c r="I13" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="67"/>
+      <c r="J13" s="127"/>
       <c r="K13" s="22" t="s">
         <v>29</v>
       </c>
@@ -1780,10 +2965,11 @@
       <c r="M13" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="N13" s="69"/>
-      <c r="O13" s="58"/>
-    </row>
-    <row r="14" spans="1:16" s="26" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N13" s="129"/>
+      <c r="O13" s="116"/>
+      <c r="P13" s="118"/>
+    </row>
+    <row r="14" spans="1:17" s="26" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -1799,25 +2985,26 @@
       <c r="M14" s="25"/>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P14" s="23"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:J5"/>
     <mergeCell ref="K4:M5"/>
-    <mergeCell ref="N4:O5"/>
+    <mergeCell ref="N4:P5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:J7"/>
     <mergeCell ref="K6:M9"/>
-    <mergeCell ref="N6:O9"/>
+    <mergeCell ref="N6:P9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:J9"/>
     <mergeCell ref="A12:A13"/>
@@ -1826,9 +3013,10 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N10:P10"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="N12:N13"/>
   </mergeCells>
@@ -1847,7 +3035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6DA28D-9BA1-40F8-AF7E-6A559A47F027}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1901,12 +3089,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF44DDF-8ED1-4864-8590-37C9E8A63962}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,6 +3105,16 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
@@ -1924,7 +3122,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ActivityName xmlns="90971145-0e3f-401e-a533-b224f340d0bb" xsi:nil="true"/>
@@ -2156,7 +3354,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ISO Document" ma:contentTypeID="0x01010086934EBC94246946B23F5DD9F27BF11F00B2FADA0FA4969F4D83190839948D67F5" ma:contentTypeVersion="51" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="fe874aa8cdea4475ac883b87bea1de2d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90971145-0e3f-401e-a533-b224f340d0bb" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="55f8bd73-a108-495f-bfbd-f04bb513be94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f645651e80efe6f1c815ba2641e5d38c" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="90971145-0e3f-401e-a533-b224f340d0bb"/>
@@ -2747,17 +3945,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1BCF8DD-F64D-40E2-9E31-964B85018AAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93835A57-0014-4DA9-A2E8-6D1E26215A39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2765,7 +3961,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B36565D-48F5-4A14-839C-2DA862D8E795}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2776,7 +3972,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70866C74-89F7-4E96-902B-60E69D0AD1FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2794,12 +3990,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1BCF8DD-F64D-40E2-9E31-964B85018AAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>